<commit_message>
Added scanning page. Updated total ugc count to use SteamDB top 100 games
</commit_message>
<xml_diff>
--- a/SteamWebScraper/UGCOfWorkshopMonth/UGCOfWorkshopMonth 2024-2.xlsx
+++ b/SteamWebScraper/UGCOfWorkshopMonth/UGCOfWorkshopMonth 2024-2.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megaz\Documents\CurveWorkshopTools\SteamWebScraper\UGCOfWorkshopMonth\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F87CD4-14FA-45B1-A8FA-79945104D144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="690" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024 2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="60">
   <si>
     <t>Name of the level</t>
   </si>
@@ -199,8 +205,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,25 +261,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -311,7 +326,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -345,6 +360,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -379,9 +395,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -554,14 +571,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -613,7 +640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -642,7 +669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -671,7 +698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -700,7 +727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -726,7 +753,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -752,7 +779,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -778,7 +805,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -804,7 +831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -830,7 +857,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -856,7 +883,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -882,7 +909,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -906,6 +933,318 @@
       </c>
       <c r="H13" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>4644</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="5">
+        <v>45300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>1284</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="5">
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>2609</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="5">
+        <v>45296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>3610</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="5">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>564</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="5">
+        <v>45305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>677</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="5">
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20">
+        <v>175</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="5">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>1288</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="5">
+        <v>45300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22">
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="5">
+        <v>45311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23">
+        <v>92</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="5">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <v>418</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="5">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25">
+        <v>76</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="5">
+        <v>45318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>